<commit_message>
more process to input and output: out title.
</commit_message>
<xml_diff>
--- a/input/国美后台数据/美票宝投资总表（32）.xlsx
+++ b/input/国美后台数据/美票宝投资总表（32）.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20388" windowHeight="8376" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20388" windowHeight="8376"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,49 +17,61 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
+    <t>WJRTB-MYLC-RYBL-32</t>
+  </si>
+  <si>
+    <t>3130005142073297</t>
+  </si>
+  <si>
+    <t>融通宝系列产品投资/清算总表（YYYY/MM/DD）</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <t>序号</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>产品编号</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>票号</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>募集成功日期</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>起息日</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>到期日</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>存续天数</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>预期年化收益率</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>投资人次</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>投资金额</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>投资收益</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>本息合计</t>
-  </si>
-  <si>
-    <t>WJRTB-MYLC-RYBL-32</t>
-  </si>
-  <si>
-    <t>3130005142073297</t>
-  </si>
-  <si>
-    <t>融通宝系列产品投资/清算总表（YYYY/MM/DD）</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -69,7 +81,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -84,6 +96,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -91,6 +104,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -110,18 +124,21 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -200,13 +217,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -477,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -498,56 +515,56 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.399999999999999">
       <c r="A1" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+        <v>2</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="15.6">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.8">
@@ -555,10 +572,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4">
         <v>42837</v>
@@ -705,17 +722,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="19">
+      <c r="A1" s="17">
         <v>42850</v>
       </c>
     </row>

</xml_diff>